<commit_message>
tao 2 trang chi tiet
</commit_message>
<xml_diff>
--- a/BTLproject/data_test/fake_dslop.xlsx
+++ b/BTLproject/data_test/fake_dslop.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\QuanLyTrucNhatSinhVienHaUI\BTLproject\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FE4410-DE0C-40F6-8B96-11E5C8E613F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7788" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -767,7 +768,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1065,143 +1066,143 @@
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1516,16 +1517,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1538,514 +1539,514 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="28">
         <v>2021604178</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="29">
         <v>2021603956</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="29">
         <v>2021600229</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="29">
         <v>2021603356</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="29">
         <v>2021603314</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="A7" s="29">
         <v>2021601030</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="A8" s="29">
         <v>2021602863</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="A9" s="29">
         <v>2021600743</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="A10" s="29">
         <v>2021603238</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="29">
         <v>2021600594</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+      <c r="A12" s="29">
         <v>2021600910</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="A13" s="29">
         <v>2021607799</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+      <c r="A14" s="29">
         <v>2021608233</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
+      <c r="A15" s="30">
         <v>2021608148</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
+      <c r="A16" s="31">
         <v>2021608453</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="29">
         <v>2021607789</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+      <c r="A18" s="29">
         <v>2021608007</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+      <c r="A19" s="29">
         <v>2021605945</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="29">
         <v>2021607358</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="A21" s="29">
         <v>2021605406</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+      <c r="A22" s="29">
         <v>2021608319</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="8">
+      <c r="A23" s="32">
         <v>2021603837</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
+      <c r="A24" s="29">
         <v>2021607023</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+      <c r="A25" s="29">
         <v>2021600415</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
+      <c r="A26" s="29">
         <v>2021601086</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
+      <c r="A27" s="29">
         <v>2021602078</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
+      <c r="A28" s="29">
         <v>2020605724</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
+      <c r="A29" s="29">
         <v>2023600179</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
+      <c r="A30" s="29">
         <v>2021602785</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
+      <c r="A31" s="29">
         <v>2021608108</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
+      <c r="A32" s="29">
         <v>2021608607</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3">
+      <c r="A33" s="29">
         <v>2021608679</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
+      <c r="A34" s="29">
         <v>2021603887</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3">
+      <c r="A35" s="29">
         <v>2021603587</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3">
+      <c r="A36" s="29">
         <v>2021606076</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3">
+      <c r="A37" s="29">
         <v>2021608263</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3">
+      <c r="A38" s="29">
         <v>2021608272</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
+      <c r="A39" s="29">
         <v>2021607947</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="10">
+      <c r="A40" s="33">
         <v>2021608636</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="10">
+      <c r="A41" s="33">
         <v>2021608013</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="10">
+      <c r="A42" s="33">
         <v>2021608464</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="3">
+      <c r="A43" s="29">
         <v>2021605707</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="3">
+      <c r="A44" s="29">
         <v>2021605430</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="3">
+      <c r="A45" s="29">
         <v>2021605176</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="3">
+      <c r="A46" s="29">
         <v>2021607814</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="10">
+      <c r="A47" s="33">
         <v>2021607917</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="3">
+      <c r="A48" s="29">
         <v>2021607975</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3">
+      <c r="A49" s="29">
         <v>2021602931</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="3">
+      <c r="A50" s="29">
         <v>2021601675</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="3">
+      <c r="A51" s="29">
         <v>2019600428</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="3">
+      <c r="A52" s="29">
         <v>2021606348</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3">
+      <c r="A53" s="29">
         <v>2021606935</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="3">
+      <c r="A54" s="29">
         <v>2021600133</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="3">
+      <c r="A55" s="29">
         <v>2021601616</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="3">
+      <c r="A56" s="29">
         <v>2021601280</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="3">
+      <c r="A57" s="29">
         <v>2021608379</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="3">
+      <c r="A58" s="29">
         <v>2021608142</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="3">
+      <c r="A59" s="29">
         <v>2021608525</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="3">
+      <c r="A60" s="29">
         <v>2021608361</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="3">
+      <c r="A61" s="29">
         <v>2021608362</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="3">
+      <c r="A62" s="29">
         <v>2021607870</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="3">
+      <c r="A63" s="29">
         <v>2021605354</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="3">
+      <c r="A64" s="29">
         <v>2021608524</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="3">
+      <c r="A65" s="29">
         <v>2021607990</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2056,16 +2057,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2078,614 +2079,614 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="41">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="41">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="41">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13">
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="41">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="42">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="42">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
+    <row r="9" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="42">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="42">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15">
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="42">
         <v>10</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="17">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="43">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="17">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="43">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="17">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="43">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="17">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="43">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17">
+    <row r="16" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="43">
         <v>15</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17">
+    <row r="17" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="43">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="43">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="43">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="17">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="43">
         <v>19</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19">
+    <row r="21" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="23">
         <v>20</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19">
+    <row r="22" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23">
         <v>21</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19">
+    <row r="23" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="23">
         <v>22</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19">
+    <row r="24" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="23">
         <v>23</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19">
+    <row r="25" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="23">
         <v>24</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19">
+    <row r="26" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="23">
         <v>25</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="19">
+    <row r="27" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="23">
         <v>26</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="19">
+    <row r="28" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="23">
         <v>27</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="19">
+    <row r="29" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="23">
         <v>28</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19">
+    <row r="30" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="23">
         <v>29</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23">
+      <c r="A31" s="45">
         <v>30</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="45" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-    </row>
-    <row r="33" spans="1:2" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="20">
+      <c r="A32" s="46"/>
+      <c r="B32" s="46"/>
+    </row>
+    <row r="33" spans="1:2" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="44">
         <v>31</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20">
+    <row r="34" spans="1:2" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="44">
         <v>32</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="20">
+    <row r="35" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="44">
         <v>33</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="20">
+    <row r="36" spans="1:2" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="44">
         <v>34</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20">
+    <row r="37" spans="1:2" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="44">
         <v>35</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="17">
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="43">
         <v>36</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="17">
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="43">
         <v>37</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="17">
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="43">
         <v>38</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="17">
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="43">
         <v>39</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="17">
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="43">
         <v>40</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="17">
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="43">
         <v>41</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="17">
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="43">
         <v>42</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="17">
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="43">
         <v>43</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="17">
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="43">
         <v>44</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="17">
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="43">
         <v>45</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="17">
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="43">
         <v>46</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="17">
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="43">
         <v>47</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="17">
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="43">
         <v>48</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="17">
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="43">
         <v>49</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="17">
+    <row r="52" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="43">
         <v>50</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="17">
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="43">
         <v>51</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="17">
+    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="43">
         <v>52</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="17">
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="43">
         <v>53</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="17">
+    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="43">
         <v>54</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="17">
+    <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="43">
         <v>55</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="17">
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="43">
         <v>56</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="17">
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="43">
         <v>57</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="17">
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="43">
         <v>58</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="17">
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="43">
         <v>59</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="17">
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="43">
         <v>60</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="17">
+    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="43">
         <v>61</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="17">
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="43">
         <v>62</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="17">
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="43">
         <v>63</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="17">
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="43">
         <v>64</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="17">
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="43">
         <v>65</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="17">
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="43">
         <v>66</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="17">
+    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="43">
         <v>67</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="17">
+    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="43">
         <v>68</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="17">
+    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="43">
         <v>69</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="17">
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="43">
         <v>70</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="17">
+    <row r="73" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="43">
         <v>71</v>
       </c>
-      <c r="B73" s="18" t="s">
+      <c r="B73" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="17">
+    <row r="74" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="43">
         <v>72</v>
       </c>
-      <c r="B74" s="18" t="s">
+      <c r="B74" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="17">
+    <row r="75" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="43">
         <v>73</v>
       </c>
-      <c r="B75" s="18" t="s">
+      <c r="B75" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="17">
+    <row r="76" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="43">
         <v>74</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="17">
+    <row r="77" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="43">
         <v>75</v>
       </c>
-      <c r="B77" s="18" t="s">
+      <c r="B77" s="9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="17">
+    <row r="78" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="43">
         <v>76</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="9" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2699,512 +2700,512 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24">
         <v>2020603405</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="20" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42">
+    <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="25">
         <v>2021608319</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="21" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="44">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="26">
         <v>2021605960</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="21" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="44">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
         <v>2021605672</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="21" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45">
+    <row r="5" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27">
         <v>2021605179</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="22" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45">
+    <row r="6" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27">
         <v>2021606104</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="22" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="45">
+    <row r="7" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="27">
         <v>2021605356</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="22" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="45">
+    <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="27">
         <v>2021600647</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="22" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="44">
+    <row r="9" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="26">
         <v>2021605982</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="21" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="44">
+    <row r="10" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="26">
         <v>2021607913</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="21" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44">
+    <row r="11" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="26">
         <v>2021607155</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="21" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="44">
+      <c r="A12" s="26">
         <v>2021608392</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="21" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="45">
+      <c r="A13" s="27">
         <v>2017600653</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="22" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="45">
+    <row r="14" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="27">
         <v>2017605909</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="22" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="44">
+    <row r="15" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26">
         <v>2021604079</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="44">
+    <row r="16" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="26">
         <v>2021603749</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="21" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44">
+    <row r="17" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="26">
         <v>2021600266</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="21" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="44">
+    <row r="18" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="26">
         <v>2021601149</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="21" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="44">
+    <row r="19" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="26">
         <v>2020604222</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="21" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="45">
+    <row r="20" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="27">
         <v>2021601846</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="22" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="45">
+    <row r="21" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="27">
         <v>2021601120</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="22" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="45">
+    <row r="22" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="27">
         <v>2021601817</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="22" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="45">
+    <row r="23" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="27">
         <v>2021600211</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="22" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="45">
+      <c r="A24" s="27">
         <v>2021601311</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="22" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="44">
+    <row r="25" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="26">
         <v>2021605532</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="21" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="44">
+    <row r="26" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="26">
         <v>2021604175</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="21" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="44">
+    <row r="27" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="26">
         <v>2021604268</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="21" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="44">
+    <row r="28" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="26">
         <v>2021603631</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="21" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="44">
+    <row r="29" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="26">
         <v>2021604432</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="45">
+    <row r="30" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="27">
         <v>2021603085</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="22" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="45">
+    <row r="31" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="27">
         <v>2021601713</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="22" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="45">
+    <row r="32" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="27">
         <v>2021602931</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="22" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="45">
+    <row r="33" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="27">
         <v>2021603110</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="45">
+    <row r="34" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="27">
         <v>2021602873</v>
       </c>
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="22" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="44">
+    <row r="35" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="26">
         <v>2020602536</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="21" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="44">
+    <row r="36" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="26">
         <v>2021605406</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="21" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="44">
+    <row r="37" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="26">
         <v>2020605502</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="21" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="45">
+      <c r="A38" s="27">
         <v>2020605565</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="22" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="45">
+    <row r="39" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="27">
         <v>2021602145</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="22" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="44">
+    <row r="40" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="26">
         <v>2020601842</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="21" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="44">
+    <row r="41" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="26">
         <v>2020608156</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="21" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="44">
+    <row r="42" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="26">
         <v>2021606718</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="21" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="44">
+    <row r="43" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="26">
         <v>2020605970</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="21" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="45">
+    <row r="44" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="27">
         <v>2021603232</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="22" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="45">
+    <row r="45" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="27">
         <v>2021604025</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="22" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="45">
+    <row r="46" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="27">
         <v>2021605437</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="22" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="44">
+    <row r="47" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="26">
         <v>2021602661</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="21" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="44">
+    <row r="48" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="26">
         <v>2021601236</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="21" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="44">
+    <row r="49" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="26">
         <v>2021606931</v>
       </c>
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="21" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="44">
+      <c r="A50" s="26">
         <v>2021605103</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="21" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="45">
+    <row r="51" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="27">
         <v>2020603093</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="22" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="45">
+      <c r="A52" s="27">
         <v>2020606605</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="22" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="44">
+    <row r="53" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="26">
         <v>2019605033</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="44">
+    <row r="54" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="26">
         <v>2021600594</v>
       </c>
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="21" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="44">
+    <row r="55" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="26">
         <v>2021604271</v>
       </c>
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="21" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="44">
+    <row r="56" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="26">
         <v>2021606265</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="21" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="44">
+    <row r="57" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="26">
         <v>2020605304</v>
       </c>
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="21" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="45">
+    <row r="58" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="27">
         <v>2021601915</v>
       </c>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="22" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="45">
+    <row r="59" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="27">
         <v>2021601764</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="22" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="45">
+    <row r="60" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="27">
         <v>2021602947</v>
       </c>
-      <c r="B60" s="46" t="s">
+      <c r="B60" s="22" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="45">
+    <row r="61" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="27">
         <v>2021605945</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="22" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="45">
+    <row r="62" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="27">
         <v>2021607358</v>
       </c>
-      <c r="B62" s="46" t="s">
+      <c r="B62" s="22" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3214,588 +3215,589 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B71"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="25">
+    <row r="1" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="34">
         <v>2020604075</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="27">
+    <row r="2" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="35">
         <v>2020607555</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="27">
+    <row r="3" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="35">
         <v>2020608221</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="27">
+    <row r="4" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="35">
         <v>2020604294</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="13" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="29">
+    <row r="5" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="36">
         <v>2020605626</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="31">
+    <row r="6" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="37">
         <v>2020606546</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="31">
+    <row r="7" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="37">
         <v>2021606462</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="31">
+    <row r="8" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="37">
         <v>2020604941</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="31">
+    <row r="9" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="37">
         <v>2020604119</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="33">
+    <row r="10" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="38">
         <v>2019605772</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="27">
+    <row r="11" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="35">
         <v>2020603230</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="13" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="27">
+    <row r="12" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="35">
         <v>2020602926</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="27">
+    <row r="13" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="35">
         <v>2020602017</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="27">
+    <row r="14" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="35">
         <v>2020603896</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="29">
+    <row r="15" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="36">
         <v>2021608308</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="17" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="31">
+    <row r="16" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="37">
         <v>2021602430</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="31">
+    <row r="17" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="37">
         <v>2021600415</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="31">
+    <row r="18" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="37">
         <v>2021604180</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="31">
+    <row r="19" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="37">
         <v>2021601944</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="33">
+    <row r="20" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="38">
         <v>2020603002</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="16" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="27">
+    <row r="21" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="35">
         <v>2021607725</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="27">
+    <row r="22" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="35">
         <v>2021603611</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="27">
+    <row r="23" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="35">
         <v>2021607262</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="27">
+    <row r="24" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="35">
         <v>2021604574</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="13" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="36">
+    <row r="25" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="39">
         <v>2021608512</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="31">
+    <row r="26" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="37">
         <v>2021600173</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="15" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="31">
+    <row r="27" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="37">
         <v>2021600258</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="31">
+    <row r="28" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="37">
         <v>2021600455</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="38">
+    <row r="29" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="40">
         <v>2021601128</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="33">
+    <row r="30" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="38">
         <v>2021604722</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="16" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="27">
+    <row r="31" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="35">
         <v>2021603421</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="13" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="27">
+    <row r="32" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="35">
         <v>2021604905</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="27">
+    <row r="33" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="35">
         <v>2021606577</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="27">
+    <row r="34" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="35">
         <v>2021604271</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="29">
+    <row r="35" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="36">
         <v>2021605125</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="19" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="31">
+    <row r="36" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="37">
         <v>2021606265</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="31">
+    <row r="37" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="37">
         <v>2021605945</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="31">
+    <row r="38" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="37">
         <v>2021601999</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="31">
+    <row r="39" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="37">
         <v>2021608319</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="33">
+    <row r="40" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="38">
         <v>2021607023</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="27">
+    <row r="41" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="35">
         <v>2020607370</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="27">
+    <row r="42" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="35">
         <v>2021600222</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="27">
+    <row r="43" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="35">
         <v>2021602720</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="27">
+    <row r="44" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="35">
         <v>2021600878</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="29">
+    <row r="45" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="36">
         <v>2021602842</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="31">
+    <row r="46" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="37">
         <v>2020602706</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="31">
+    <row r="47" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="37">
         <v>2020601514</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="31">
+    <row r="48" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="37">
         <v>2020605740</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="31">
+    <row r="49" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="37">
         <v>2020606033</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="33">
+    <row r="50" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="38">
         <v>2020601411</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="16" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="27">
+    <row r="51" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="35">
         <v>2021606977</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="13" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="27">
+    <row r="52" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="35">
         <v>2021605672</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="13" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="27">
+    <row r="53" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="35">
         <v>2021605488</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="13" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="27">
+    <row r="54" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="35">
         <v>2021606937</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="29">
+    <row r="55" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="36">
         <v>2021607126</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="19" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="31">
+    <row r="56" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="37">
         <v>2018601171</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="31">
+    <row r="57" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="37">
         <v>2021608610</v>
       </c>
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="15" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="31">
+    <row r="58" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="37">
         <v>2021602352</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="31">
+    <row r="59" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="37">
         <v>2020606243</v>
       </c>
-      <c r="B59" s="32" t="s">
+      <c r="B59" s="15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="31">
+    <row r="60" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="37">
         <v>2021603697</v>
       </c>
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="33">
+    <row r="61" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="38">
         <v>2021606385</v>
       </c>
-      <c r="B61" s="34" t="s">
+      <c r="B61" s="16" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="27">
+    <row r="62" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="35">
         <v>2020600300</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="27">
+    <row r="63" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="35">
         <v>2020601068</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="13" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="27">
+    <row r="64" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="35">
         <v>2021605938</v>
       </c>
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="27">
+    <row r="65" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="35">
         <v>2020601183</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="B65" s="13" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="29">
+    <row r="66" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="36">
         <v>2019603933</v>
       </c>
-      <c r="B66" s="39" t="s">
+      <c r="B66" s="19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="31">
+    <row r="67" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="37">
         <v>2021602516</v>
       </c>
-      <c r="B67" s="32" t="s">
+      <c r="B67" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="31">
+    <row r="68" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="37">
         <v>2021602692</v>
       </c>
-      <c r="B68" s="32" t="s">
+      <c r="B68" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="31">
+    <row r="69" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="37">
         <v>2021602863</v>
       </c>
-      <c r="B69" s="32" t="s">
+      <c r="B69" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="31">
+    <row r="70" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="37">
         <v>2021602931</v>
       </c>
-      <c r="B70" s="32" t="s">
+      <c r="B70" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="33">
+    <row r="71" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="38">
         <v>2020602647</v>
       </c>
-      <c r="B71" s="34" t="s">
+      <c r="B71" s="16" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>